<commit_message>
Update ERP 시스템 표준 통신 프로토콜 정의_2021_10_28.xlsx
</commit_message>
<xml_diff>
--- a/protocol/ERP 시스템 표준 통신 프로토콜 정의_2021_10_28.xlsx
+++ b/protocol/ERP 시스템 표준 통신 프로토콜 정의_2021_10_28.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoikazto/Desktop/git/asw-Document/protocol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoikazto/Desktop/git/Erp-Document/protocol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D24C0-B2C4-7E4B-9FCA-506922E51230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326569CD-BD15-CB4E-8E71-315249FC05DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="46440" windowHeight="31540" activeTab="2" xr2:uid="{48572F7A-0ACE-C246-B590-9F1E9A03BAAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{48572F7A-0ACE-C246-B590-9F1E9A03BAAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2934" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2945" uniqueCount="223">
   <si>
     <t>Sender</t>
   </si>
@@ -906,6 +906,14 @@
   </si>
   <si>
     <t>토큰 만료일 (재로그인)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로토콜 번호(0x43)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>,.,.kl;oppl;.//;/;;/</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1242,16 +1250,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1907,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BFF69C-9C3A-B345-A9B8-38043CBDF4E2}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A8" zoomScale="131" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1918,20 +1926,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="19" thickBot="1">
       <c r="A4" s="26" t="s">
@@ -2005,7 +2013,7 @@
       <c r="A8" s="25">
         <v>0.6</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="32">
         <v>44498</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -2157,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3088A680-D3EE-E74F-A31D-C834569A6AFF}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2343,7 +2351,7 @@
       <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -2366,7 +2374,7 @@
       <c r="N7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="P7" s="10" t="s">
@@ -2389,12 +2397,10 @@
       <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="F8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="10"/>
       <c r="J8" s="7">
         <v>3</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>10</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>13</v>
@@ -2434,10 +2440,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="J9" s="7">
         <v>4</v>
@@ -2455,10 +2461,10 @@
         <v>10</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2478,10 +2484,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="J10" s="7">
         <v>5</v>
@@ -2499,10 +2505,10 @@
         <v>10</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2522,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>13</v>
@@ -2543,139 +2549,139 @@
         <v>10</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="7">
+        <v>7</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="J14" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="J15" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="L15" s="2"/>
+      <c r="M15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="J16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P16" s="7" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="7">
-        <v>1</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="7">
-        <v>1</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>9</v>
@@ -2689,14 +2695,14 @@
       <c r="E17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>17</v>
+      <c r="F17" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>12</v>
@@ -2710,8 +2716,8 @@
       <c r="N17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>17</v>
+      <c r="O17" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>13</v>
@@ -2719,7 +2725,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>9</v>
@@ -2733,14 +2739,14 @@
       <c r="E18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>33</v>
+      <c r="F18" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>12</v>
@@ -2754,16 +2760,16 @@
       <c r="N18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="10" t="s">
-        <v>33</v>
+      <c r="O18" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="7">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>9</v>
@@ -2778,13 +2784,13 @@
         <v>10</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="J19" s="7">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>12</v>
@@ -2799,15 +2805,15 @@
         <v>10</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P19" s="11" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="7">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>9</v>
@@ -2822,13 +2828,13 @@
         <v>10</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J20" s="7">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>12</v>
@@ -2843,7 +2849,7 @@
         <v>10</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>8</v>
@@ -2851,7 +2857,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>9</v>
@@ -2872,7 +2878,7 @@
         <v>8</v>
       </c>
       <c r="J21" s="7">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>12</v>
@@ -2884,10 +2890,10 @@
         <v>9</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>8</v>
@@ -2895,7 +2901,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="7">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>9</v>
@@ -2916,7 +2922,7 @@
         <v>8</v>
       </c>
       <c r="J22" s="7">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>12</v>
@@ -2931,7 +2937,7 @@
         <v>10</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>8</v>
@@ -2939,7 +2945,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="7">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>9</v>
@@ -2960,7 +2966,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="7">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>12</v>
@@ -2983,7 +2989,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>9</v>
@@ -3004,7 +3010,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="7">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>12</v>
@@ -3027,7 +3033,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="7">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>9</v>
@@ -3048,7 +3054,7 @@
         <v>8</v>
       </c>
       <c r="J25" s="7">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>12</v>
@@ -3071,7 +3077,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="7">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>9</v>
@@ -3092,7 +3098,7 @@
         <v>8</v>
       </c>
       <c r="J26" s="7">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>12</v>
@@ -3115,7 +3121,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>9</v>
@@ -3130,13 +3136,13 @@
         <v>10</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="J27" s="7">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>12</v>
@@ -3151,15 +3157,15 @@
         <v>10</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="P27" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>9</v>
@@ -3174,7 +3180,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>13</v>
@@ -3195,132 +3201,132 @@
         <v>10</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="P28" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" t="s">
-        <v>36</v>
+    <row r="29" spans="1:16">
+      <c r="A29" s="7">
+        <v>6</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="7">
+        <v>6</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="J32" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="J33" t="s">
         <v>25</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N32" s="7"/>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="L33" s="2"/>
+      <c r="M33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" s="7"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K33" s="5" t="s">
+      <c r="J34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="6" t="s">
+      <c r="L34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N33" s="7" t="s">
+      <c r="N34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O33" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P33" s="7" t="s">
+      <c r="P34" s="7" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="7">
-        <v>1</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="7">
-        <v>1</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O34" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>9</v>
@@ -3334,14 +3340,14 @@
       <c r="E35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="12" t="s">
-        <v>17</v>
+      <c r="F35" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J35" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>12</v>
@@ -3355,8 +3361,8 @@
       <c r="N35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O35" s="12" t="s">
-        <v>17</v>
+      <c r="O35" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="P35" s="7" t="s">
         <v>13</v>
@@ -3364,7 +3370,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>9</v>
@@ -3378,14 +3384,14 @@
       <c r="E36" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>34</v>
+      <c r="F36" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>13</v>
       </c>
       <c r="J36" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>12</v>
@@ -3399,8 +3405,8 @@
       <c r="N36" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O36" s="10" t="s">
-        <v>34</v>
+      <c r="O36" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="P36" s="7" t="s">
         <v>13</v>
@@ -3408,7 +3414,7 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="7">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>9</v>
@@ -3423,13 +3429,13 @@
         <v>10</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>8</v>
+        <v>221</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="J37" s="7">
-        <v>4.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>12</v>
@@ -3444,7 +3450,7 @@
         <v>10</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>37</v>
+        <v>221</v>
       </c>
       <c r="P37" s="7" t="s">
         <v>13</v>
@@ -3452,7 +3458,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="7">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>9</v>
@@ -3467,13 +3473,13 @@
         <v>10</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J38" s="7">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>12</v>
@@ -3488,15 +3494,15 @@
         <v>10</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="P38" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>9</v>
@@ -3517,7 +3523,7 @@
         <v>8</v>
       </c>
       <c r="J39" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>12</v>
@@ -3532,15 +3538,15 @@
         <v>10</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="P39" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="7">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>9</v>
@@ -3560,10 +3566,31 @@
       <c r="G40" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="J40" s="7">
+        <v>6</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="7">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>9</v>
@@ -3586,7 +3613,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>9</v>
@@ -3609,7 +3636,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="7">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>9</v>
@@ -3632,7 +3659,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="7">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>9</v>
@@ -3655,7 +3682,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>9</v>
@@ -3670,15 +3697,15 @@
         <v>10</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>9</v>
@@ -3693,15 +3720,39 @@
         <v>10</v>
       </c>
       <c r="F46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="7">
+        <v>6</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G47" s="10" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3710,8 +3761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8262301-E68F-1C43-B727-9D392BE05D7B}">
   <dimension ref="A1:AI126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q64" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y95" sqref="Y95"/>
+    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3843,48 +3894,48 @@
       </c>
     </row>
     <row r="20" spans="1:35">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
       <c r="E20" t="s">
         <v>56</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="32" t="s">
+      <c r="J20" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
       <c r="N20" t="s">
         <v>56</v>
       </c>
       <c r="O20" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="32" t="s">
+      <c r="S20" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
+      <c r="T20" s="34"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="34"/>
       <c r="W20" t="s">
         <v>56</v>
       </c>
       <c r="X20" t="s">
         <v>58</v>
       </c>
-      <c r="AB20" s="32" t="s">
+      <c r="AB20" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="AC20" s="32"/>
-      <c r="AD20" s="32"/>
-      <c r="AE20" s="32"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="34"/>
+      <c r="AE20" s="34"/>
       <c r="AF20" t="s">
         <v>56</v>
       </c>
@@ -4900,24 +4951,24 @@
       <c r="Q34" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="S34" s="32" t="s">
+      <c r="S34" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
+      <c r="T34" s="34"/>
+      <c r="U34" s="34"/>
+      <c r="V34" s="34"/>
       <c r="W34" t="s">
         <v>56</v>
       </c>
       <c r="X34" t="s">
         <v>58</v>
       </c>
-      <c r="AB34" s="32" t="s">
+      <c r="AB34" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="AC34" s="32"/>
-      <c r="AD34" s="32"/>
-      <c r="AE34" s="32"/>
+      <c r="AC34" s="34"/>
+      <c r="AD34" s="34"/>
+      <c r="AE34" s="34"/>
       <c r="AF34" t="s">
         <v>56</v>
       </c>
@@ -5037,12 +5088,12 @@
       </c>
     </row>
     <row r="37" spans="1:35">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
       <c r="E37" t="s">
         <v>56</v>
       </c>
@@ -5315,12 +5366,12 @@
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="14"/>
-      <c r="J41" s="32" t="s">
+      <c r="J41" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
       <c r="N41" t="s">
         <v>56</v>
       </c>
@@ -5847,12 +5898,12 @@
       <c r="Q48" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="S48" s="32" t="s">
+      <c r="S48" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T48" s="32"/>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
+      <c r="T48" s="34"/>
+      <c r="U48" s="34"/>
+      <c r="V48" s="34"/>
       <c r="W48" t="s">
         <v>56</v>
       </c>
@@ -6133,12 +6184,12 @@
         <v>1</v>
       </c>
       <c r="W52" s="7"/>
-      <c r="AB52" s="32" t="s">
+      <c r="AB52" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="AC52" s="32"/>
-      <c r="AD52" s="32"/>
-      <c r="AE52" s="32"/>
+      <c r="AC52" s="34"/>
+      <c r="AD52" s="34"/>
+      <c r="AE52" s="34"/>
       <c r="AF52" t="s">
         <v>56</v>
       </c>
@@ -6632,12 +6683,12 @@
       </c>
     </row>
     <row r="62" spans="1:35">
-      <c r="S62" s="32" t="s">
+      <c r="S62" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T62" s="32"/>
-      <c r="U62" s="32"/>
-      <c r="V62" s="32"/>
+      <c r="T62" s="34"/>
+      <c r="U62" s="34"/>
+      <c r="V62" s="34"/>
       <c r="W62" t="s">
         <v>56</v>
       </c>
@@ -6808,25 +6859,25 @@
       </c>
     </row>
     <row r="69" spans="1:34">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="32"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="O69" s="32"/>
-      <c r="P69" s="32"/>
-      <c r="Q69" s="32"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="34"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="34"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34"/>
+      <c r="Q69" s="34"/>
       <c r="S69" s="7">
         <v>1</v>
       </c>
@@ -6954,11 +7005,11 @@
       <c r="Z73" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AD73" s="31" t="s">
+      <c r="AD73" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="AE73" s="31"/>
-      <c r="AF73" s="31"/>
+      <c r="AE73" s="33"/>
+      <c r="AF73" s="33"/>
     </row>
     <row r="74" spans="1:34">
       <c r="A74" t="s">
@@ -6981,36 +7032,36 @@
       </c>
     </row>
     <row r="82" spans="1:26" ht="19">
-      <c r="A82" s="32" t="s">
+      <c r="A82" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
       <c r="E82" t="s">
         <v>56</v>
       </c>
       <c r="F82" t="s">
         <v>57</v>
       </c>
-      <c r="J82" s="32" t="s">
+      <c r="J82" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="K82" s="32"/>
-      <c r="L82" s="32"/>
-      <c r="M82" s="32"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+      <c r="M82" s="34"/>
       <c r="N82" t="s">
         <v>56</v>
       </c>
       <c r="O82" t="s">
         <v>57</v>
       </c>
-      <c r="S82" s="32" t="s">
+      <c r="S82" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="T82" s="32"/>
-      <c r="U82" s="32"/>
-      <c r="V82" s="32"/>
+      <c r="T82" s="34"/>
+      <c r="U82" s="34"/>
+      <c r="V82" s="34"/>
       <c r="W82" t="s">
         <v>56</v>
       </c>
@@ -7709,12 +7760,12 @@
       <c r="W95" s="7"/>
     </row>
     <row r="96" spans="1:26">
-      <c r="J96" s="32" t="s">
+      <c r="J96" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="K96" s="32"/>
-      <c r="L96" s="32"/>
-      <c r="M96" s="32"/>
+      <c r="K96" s="34"/>
+      <c r="L96" s="34"/>
+      <c r="M96" s="34"/>
       <c r="N96" t="s">
         <v>56</v>
       </c>
@@ -7841,12 +7892,12 @@
       <c r="J99" t="s">
         <v>61</v>
       </c>
-      <c r="AB99" s="32" t="s">
+      <c r="AB99" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="AC99" s="32"/>
-      <c r="AD99" s="32"/>
-      <c r="AE99" s="32"/>
+      <c r="AC99" s="34"/>
+      <c r="AD99" s="34"/>
+      <c r="AE99" s="34"/>
       <c r="AF99" t="s">
         <v>56</v>
       </c>
@@ -7907,12 +7958,12 @@
       <c r="Q101" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S101" s="32" t="s">
+      <c r="S101" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="T101" s="32"/>
-      <c r="U101" s="32"/>
-      <c r="V101" s="32"/>
+      <c r="T101" s="34"/>
+      <c r="U101" s="34"/>
+      <c r="V101" s="34"/>
       <c r="W101" t="s">
         <v>56</v>
       </c>
@@ -8443,12 +8494,12 @@
       </c>
     </row>
     <row r="113" spans="19:35">
-      <c r="AB113" s="32" t="s">
+      <c r="AB113" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="AC113" s="32"/>
-      <c r="AD113" s="32"/>
-      <c r="AE113" s="32"/>
+      <c r="AC113" s="34"/>
+      <c r="AD113" s="34"/>
+      <c r="AE113" s="34"/>
       <c r="AF113" t="s">
         <v>56</v>
       </c>
@@ -8457,7 +8508,7 @@
       </c>
     </row>
     <row r="114" spans="19:35">
-      <c r="T114" s="33"/>
+      <c r="T114" s="31"/>
       <c r="AB114" t="s">
         <v>62</v>
       </c>
@@ -8472,17 +8523,17 @@
       <c r="AG114" s="14"/>
     </row>
     <row r="115" spans="19:35">
-      <c r="S115" s="33" t="s">
+      <c r="S115" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="U115" s="33"/>
+      <c r="U115" s="31"/>
       <c r="W115" t="s">
         <v>56</v>
       </c>
       <c r="X115" t="s">
         <v>57</v>
       </c>
-      <c r="Z115" s="33" t="s">
+      <c r="Z115" s="31" t="s">
         <v>205</v>
       </c>
       <c r="AB115" s="4" t="s">
@@ -8908,12 +8959,9 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AB113:AE113"/>
-    <mergeCell ref="J82:M82"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="J96:M96"/>
-    <mergeCell ref="AD73:AF73"/>
-    <mergeCell ref="AB99:AE99"/>
+    <mergeCell ref="A69:Q69"/>
+    <mergeCell ref="S82:V82"/>
+    <mergeCell ref="S101:V101"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="S62:V62"/>
     <mergeCell ref="A20:D20"/>
@@ -8925,9 +8973,12 @@
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="AB34:AE34"/>
     <mergeCell ref="S34:V34"/>
-    <mergeCell ref="A69:Q69"/>
-    <mergeCell ref="S82:V82"/>
-    <mergeCell ref="S101:V101"/>
+    <mergeCell ref="AB113:AE113"/>
+    <mergeCell ref="J82:M82"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="J96:M96"/>
+    <mergeCell ref="AD73:AF73"/>
+    <mergeCell ref="AB99:AE99"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8946,48 +8997,48 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
     <row r="6" spans="1:35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" t="s">
         <v>56</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
       <c r="N6" t="s">
         <v>56</v>
       </c>
       <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="S6" s="32" t="s">
+      <c r="S6" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
       <c r="W6" t="s">
         <v>56</v>
       </c>
       <c r="X6" t="s">
         <v>58</v>
       </c>
-      <c r="AB6" s="32" t="s">
+      <c r="AB6" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
       <c r="AF6" t="s">
         <v>56</v>
       </c>
@@ -9946,12 +9997,12 @@
       <c r="Z19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AB19" s="32" t="s">
+      <c r="AB19" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="AC19" s="32"/>
-      <c r="AD19" s="32"/>
-      <c r="AE19" s="32"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
       <c r="AF19" t="s">
         <v>56</v>
       </c>
@@ -9960,12 +10011,12 @@
       </c>
     </row>
     <row r="20" spans="1:35">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
       <c r="E20" t="s">
         <v>56</v>
       </c>
@@ -10477,12 +10528,12 @@
       <c r="H27" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J27" s="32" t="s">
+      <c r="J27" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
       <c r="N27" t="s">
         <v>56</v>
       </c>
@@ -10525,12 +10576,12 @@
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="14"/>
-      <c r="S28" s="32" t="s">
+      <c r="S28" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T28" s="32"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
       <c r="W28" t="s">
         <v>56</v>
       </c>
@@ -10919,12 +10970,12 @@
       <c r="Z33" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AB33" s="32" t="s">
+      <c r="AB33" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="AC33" s="32"/>
-      <c r="AD33" s="32"/>
-      <c r="AE33" s="32"/>
+      <c r="AC33" s="34"/>
+      <c r="AD33" s="34"/>
+      <c r="AE33" s="34"/>
       <c r="AF33" t="s">
         <v>56</v>
       </c>
@@ -10995,12 +11046,12 @@
       <c r="AG34" s="14"/>
     </row>
     <row r="35" spans="1:35">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
       <c r="E35" t="s">
         <v>56</v>
       </c>
@@ -11898,12 +11949,12 @@
       </c>
     </row>
     <row r="48" spans="1:35">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
       <c r="E48" t="s">
         <v>56</v>
       </c>
@@ -11948,12 +11999,12 @@
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="14"/>
-      <c r="J49" s="32" t="s">
+      <c r="J49" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
       <c r="N49" t="s">
         <v>56</v>
       </c>
@@ -12035,12 +12086,12 @@
       <c r="Q51" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S51" s="32" t="s">
+      <c r="S51" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T51" s="32"/>
-      <c r="U51" s="32"/>
-      <c r="V51" s="32"/>
+      <c r="T51" s="34"/>
+      <c r="U51" s="34"/>
+      <c r="V51" s="34"/>
       <c r="W51" t="s">
         <v>56</v>
       </c>
@@ -12612,6 +12663,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J27:M27"/>
     <mergeCell ref="J49:M49"/>
     <mergeCell ref="S51:V51"/>
     <mergeCell ref="S6:V6"/>
@@ -12619,12 +12676,6 @@
     <mergeCell ref="AB33:AE33"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="AB19:AE19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J27:M27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>